<commit_message>
Riesecuzione dei test case a fronte dell'aggiunta dell'attributo 'ID' ai tag 'section'.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
+++ b/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lavoro\FSE\Accreditamento\GitHub\GATEWAY\A1#111S3K00000000\S3K_SPA\JHIS\23.01.01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D44518-3F4F-4FA2-9525-4C624E0E5FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF9FACF-1812-4E56-A02F-6C11F1A03278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="227">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -779,15 +779,6 @@
     <t>subject_application_version: 23.01.01</t>
   </si>
   <si>
-    <t>2023-02-21T14:01:43Z</t>
-  </si>
-  <si>
-    <t>f4e1c706214ca25f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.4ada98dd048f8e8e1eb8b9cc4322eebb196b08df5245e06ac84b4d6a414eba6b.28a7fd37f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Le installazioni di JHIS non prevedono la gestione dell'iter clinico post dimissione.</t>
   </si>
   <si>
@@ -800,42 +791,12 @@
     <t>La conversione in XML verifica la presenza dei campi contrassegnati come obbligatori.</t>
   </si>
   <si>
-    <t>[ERRORE-44| codice fiscale 'ccrttc85t17l219' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]</t>
-  </si>
-  <si>
-    <t>2023-02-21T16:07:26Z</t>
-  </si>
-  <si>
     <t>[ERRORE-6| L'elemento 'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25']</t>
   </si>
   <si>
-    <t>4b8d2bee8d93e3de</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.bcf5cf611f78b74bbc30a3b3ddbe15fb98a001e6cd5bc87a661787302c5f4322.66fa29e568^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>017e57e23e3d04f3</t>
-  </si>
-  <si>
-    <t>2023-02-21T15:51:10Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.0f673ce1f9c0c0b57531eb50943a8d16996bd8682c54bfa206c18c80a7eff747.8e4f976c87^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il comune di residenza è sempre obbligatorio. Inoltre, la conversione in XML verifica la presenza dei campi contrassegnati come obbligatori.</t>
   </si>
   <si>
-    <t>2023-02-21T16:27:06Z</t>
-  </si>
-  <si>
-    <t>023042e4b89d6d1c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.46046833199dd191df888fec1fbef3f153acd219712682fe6d7fa09dde586ba6.ecafa659fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: NB]</t>
   </si>
   <si>
@@ -845,18 +806,6 @@
     <t>Il motivo del trasporto è sempre obbligatorio. Inoltre, la conversione in XML verifica la presenza dei campi contrassegnati come obbligatori.</t>
   </si>
   <si>
-    <t>d884153938b73ed7</t>
-  </si>
-  <si>
-    <t>2023-02-21T16:35:49Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.86e4b91a0e8381da6ff4a669a6a112d1d455b4912ccd6908aba8f73d055d9b47.7b49e2fab1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'extension' on element 'id' is not valid with respect to its type, 'st'.,E</t>
-  </si>
-  <si>
     <t>Il campo 'Evento' è sempre obbligatorio.. Inoltre, la conversione in XML verifica la presenza dei campi contrassegnati come obbligatori.</t>
   </si>
   <si>
@@ -869,132 +818,15 @@
     <t>[ERRORE-b30| Sezione Dimissione: l'entry/act \"Dimissione\" DEVE contenere un solo elemento 'entryRelationship' relativo all'Esito],[ERRORE-b31| Sezione Dimissione: l'entry/act/entryRelationship relativo all'Esito DEVE contenere  un elemento 'templateId' valorizzato con @root='2.16.840.1.113883.2.9.10.1.6.69'.],[ERRORE-b32| Sezione Dimissione: l'entry/act/entryRelationship relativo all'Esito DEVE contenere  un elemento 'statusCode' valorizzato con @code='completed'],[ERRORE-b33| Sezione Dimissione: l'entry/act/entryRelationship relativo all'Esito DEVE contenere  un elemento 'value' valorizzato secondo il value set \"EsitoTrattamento_VPS\" - @codeSystem='2.16.840.1.113883.2.9.6.1.54.5']</t>
   </si>
   <si>
-    <t>2023-02-21T17:10:13Z</t>
-  </si>
-  <si>
-    <t>d73f949914c2454f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.b2e177184682be6f3f1d8e2e0437c8da9a80e1caca53656a0c1d3b0bf2973517.8c86b1be62^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.54.1, Codes: Z]</t>
-  </si>
-  <si>
-    <t>2023-02-21T17:16:02Z</t>
-  </si>
-  <si>
-    <t>f3d9c577e52edc46</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.a69fb43eb33a073d12b676d0d86011793e1923f5c8acd5de93478fdc32af3ad9.e62db294f5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.54.4, Codes: 6]</t>
-  </si>
-  <si>
-    <t>2023-02-21T17:20:49Z</t>
-  </si>
-  <si>
-    <t>57fd23e6d5a9084f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.70cedeb22f1d23ed8920892faa406044900b96ec34110c1ca32f07be6d68db7a.3e4658f088^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 30000]</t>
   </si>
   <si>
-    <t>92f842d7f5f16e11</t>
-  </si>
-  <si>
-    <t>2023-02-21T17:24:55Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.b48f6e6ea357177d62edfca286febe14ef8f16f5f14c20e3aad7a9a584793192.8b8e358e84^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.e2147b8dfdd90c20e6cda46b633e929875a2fab908998fd16dab439a343104a2.8f67f79938^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>65f5d812147b9e22</t>
-  </si>
-  <si>
-    <t>2023-02-27T11:27:24Z</t>
-  </si>
-  <si>
-    <t>4af047cca30b5d6b</t>
-  </si>
-  <si>
-    <t>2023-02-27T11:46:08Z</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>2023-02-28T10:09:45Z</t>
-  </si>
-  <si>
-    <t>8eb9cc80faa49139</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.578704aefcac85e7adf375b331f1ddc81d8f2b474960ff1363e1ab05ba023cc3.dd6d9cbd29^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-28T10:20:27Z</t>
-  </si>
-  <si>
-    <t>023388e161246edf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.410572cbe44bfdffb49ddd69dcc00bfca5580c4f3b735e17021cfa6276d8e45b.a8a6934737^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-28T10:28:02Z</t>
-  </si>
-  <si>
-    <t>d54f2382e39b4d5e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.600939288b0d392dbb2721cf5e6d780979b10f5b2f850fa911a2b9a6f8bce313.3ddffd259b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[Errore-47| codice fiscale 'ccrttc85t17l219' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]</t>
   </si>
   <si>
-    <t>2023-02-28T10:37:47Z</t>
-  </si>
-  <si>
-    <t>ee0af9ed8d9b8a3d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.2707564b6217702920fae6c8c85de183637bd1fd59c301063befeb5afdd44494.5591143c46^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-28T11:00:03Z</t>
-  </si>
-  <si>
-    <t>ae99eb6f52cb2b4c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.6c758bb1276936a032486d40337319dbe94f9ec1e7f652982c41bc22808e04ba.adb9d6b3b1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>df938fea73d6e900</t>
-  </si>
-  <si>
-    <t>2023-02-28T11:10:11Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.b3682e4dfcc88c190303d9247d12fc1c2d2ca3e19deb9f6bc631cb45b437311e.ecb60cc70b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 42731]</t>
-  </si>
-  <si>
-    <t>[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del pa</t>
-  </si>
-  <si>
     <t>JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA</t>
   </si>
   <si>
@@ -1007,22 +839,187 @@
     <t>Le installazioni di JHIS non prevedono la gestione della terapia farmacologica.</t>
   </si>
   <si>
-    <t>Messaggio fornito dal gateway</t>
-  </si>
-  <si>
-    <t>2023-02-28T12:19:05Z</t>
-  </si>
-  <si>
-    <t>7fb2fc32b8549b3e</t>
-  </si>
-  <si>
-    <t>2023-02-28T12:21:49Z</t>
-  </si>
-  <si>
-    <t>38ddfcecf3a92f29</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.d23792bc593374f64e9550ec57b4df39bad922924a826e92d1cc9311488588f7.cb0224d76f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-04-04T15:14:17Z</t>
+  </si>
+  <si>
+    <t>7c5b99da8e7365d5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.ba58ea3e9ab92c9c9ec91e5b20038080ebc7bc87a778f9f02b1e83f1ae4905af.ce80a4b864^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e71701bb335f463f</t>
+  </si>
+  <si>
+    <t>2023-04-04T15:25:12Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.a98759b9cc4ecc1f11d04f219f1e89685c9b0a0872f6913561471fed8f1689fe.242cecf84f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-47| codice fiscale 'ccrttc85t17l219' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]</t>
+  </si>
+  <si>
+    <t>2023-04-04T15:34:26Z</t>
+  </si>
+  <si>
+    <t>9b77a6781d233bf5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.ce9f51df2561b5a2741f052817a8f2ebeac210442c099db092fe9ac975fc9020.8dbbe9d9f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-04T15:38:28Z</t>
+  </si>
+  <si>
+    <t>46014514b8c70c4d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.1f19a337adb6950eaf924b4918849d2b2c1ef00ce044cb38b771a0536713ae03.cc6ae7089b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-04T15:47:29Z</t>
+  </si>
+  <si>
+    <t>f24b7c94b09caf54</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.2e45760309b813022c89ffccc9da99a5c10bc26bcc18ba12eaacd6539c82487a.a815e30e96^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'extension' on element 'id' is not valid with respect to its type, 'st'.,ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'extension' on element 'id' is not valid with respect to its type, 'st'.,ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'extension' on element 'id' is not valid with respect to its type, 'st'.</t>
+  </si>
+  <si>
+    <t>2023-04-04T16:02:39Z</t>
+  </si>
+  <si>
+    <t>67608899afc6146b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.56a1b2ea5a6acf1c61769c4bdd57f6747d89d605d8a28e1b6a7ac5060126f853.8732ba96ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-04T16:08:41Z</t>
+  </si>
+  <si>
+    <t>b23842c617353dbf</t>
+  </si>
+  <si>
+    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.54.1, Codes: X]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.59233e4425c89d0dec3b5a70f35a7fefd6b18a73cea12bc0615b45e359577a7d.f1683f1aa4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.54.4, Codes: 0]</t>
+  </si>
+  <si>
+    <t>78c53bbd0b3e9dba</t>
+  </si>
+  <si>
+    <t>2023-04-04T16:14:46Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.9bf3394d7b9e190dd1ef5435bc3396007774e905cc77f8c11a17610e07ec9afc.22e752b624^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-04T16:26:27Z</t>
+  </si>
+  <si>
+    <t>07e80bdf413d9456</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.f8608eda5aec15c87b656123f6f984984e0cbd560585b3c9b30501609c0dbc14.36006402db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-04T16:30:46Z</t>
+  </si>
+  <si>
+    <t>778134e84e2f8763</t>
+  </si>
+  <si>
+    <t>Messaggio fornito dal gateway (ad es. "Il campo person_id non è valorizzato")</t>
+  </si>
+  <si>
+    <t>a159dabd3d976444</t>
+  </si>
+  <si>
+    <t>2023-04-04T16:34:41Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.0885ca9bffa46c5fa7261baf51ae6d0916a0f39bc0f4dcaeb1733fec6a1066e7.1eba2a8230^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-05T14:48:27Z</t>
+  </si>
+  <si>
+    <t>c0b9d91dc6ca4795</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.76b382f83be34b865eb3028d8f5aad13d26a8eb035ebff5280139a7880b8be35.a7e281e348^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-05T14:55:25Z</t>
+  </si>
+  <si>
+    <t>b83202f3ed8a76fb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.a143c2a93d019639e260fc236d7a280711ec0270400543cf44b6febf5c8ee904.728a5535a7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-05T14:58:15Z</t>
+  </si>
+  <si>
+    <t>8fc4a9b043fa2026</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.68db232115c936bdd878925a9189086e1dded9efed4c7e5674421bb7beac7f87.c1c8a6b993^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-05T15:00:42Z</t>
+  </si>
+  <si>
+    <t>0fc62afe58458a49</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.315045872ba55a2f5523e9c634d536228d19442d71a7be3b7e4dffac123b934e.163ebb7186^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Errore semantico.","detail":"[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
+  </si>
+  <si>
+    <t>2023-04-05T15:03:00Z</t>
+  </si>
+  <si>
+    <t>5bf5d78d980db52a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.a0d10d08ef0ec59dfca253813cd836c6ad3402627c57dd6021dc21a682d94bc3.b0de6df423^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.2f5cd45674dd6509e79c475673691619c26e59fbe770a1d677fe10c9e0e79790.faaa4a8da9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5dd3a831a740715e</t>
+  </si>
+  <si>
+    <t>2023-04-05T15:05:18Z</t>
+  </si>
+  <si>
+    <t>2023-04-05T15:07:34Z</t>
+  </si>
+  <si>
+    <t>514732719f910c4e</t>
+  </si>
+  <si>
+    <t>2023-04-05T15:09:31Z</t>
+  </si>
+  <si>
+    <t>ff9fd12634e91e3a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.c877847a32eeaa6b8b1ecbf81bbd2d18b17c58098e7815b7dcb5450b05dba37e.7cfe857e71^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1421,6 +1418,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1460,10 +1461,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1843,7 +1840,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,14 +1886,14 @@
       <c r="T1" s="8"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1914,14 +1911,14 @@
       <c r="T2" s="8"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="38" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="31"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -1939,12 +1936,12 @@
       <c r="T3" s="8"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="38" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="10"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1963,12 +1960,12 @@
       <c r="T4" s="8"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="31"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -1986,8 +1983,8 @@
       <c r="T5" s="8"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="11"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -2121,16 +2118,16 @@
         <v>20</v>
       </c>
       <c r="F10" s="18">
-        <v>44984</v>
+        <v>45021</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="J10" s="20" t="s">
         <v>36</v>
@@ -2172,7 +2169,7 @@
         <v>124</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
@@ -2210,7 +2207,7 @@
         <v>124</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
@@ -2248,7 +2245,7 @@
         <v>124</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
@@ -2279,16 +2276,16 @@
         <v>29</v>
       </c>
       <c r="F14" s="18">
-        <v>44978</v>
+        <v>45020</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>36</v>
@@ -2330,7 +2327,7 @@
         <v>124</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
@@ -2368,7 +2365,7 @@
         <v>124</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
@@ -2406,7 +2403,7 @@
         <v>124</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L17" s="20"/>
       <c r="M17" s="20"/>
@@ -2437,16 +2434,16 @@
         <v>38</v>
       </c>
       <c r="F18" s="18">
-        <v>44984</v>
+        <v>45021</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="J18" s="20" t="s">
         <v>36</v>
@@ -2459,13 +2456,13 @@
         <v>36</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="O18" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P18" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q18" s="20"/>
       <c r="R18" s="23"/>
@@ -2491,16 +2488,16 @@
         <v>40</v>
       </c>
       <c r="F19" s="18">
-        <v>44985</v>
+        <v>45020</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="J19" s="20" t="s">
         <v>36</v>
@@ -2513,13 +2510,13 @@
         <v>36</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="O19" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P19" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q19" s="20"/>
       <c r="R19" s="23"/>
@@ -2545,16 +2542,16 @@
         <v>42</v>
       </c>
       <c r="F20" s="18">
-        <v>44985</v>
+        <v>45021</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="J20" s="20" t="s">
         <v>36</v>
@@ -2567,13 +2564,13 @@
         <v>36</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>218</v>
+        <v>162</v>
       </c>
       <c r="O20" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P20" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q20" s="20"/>
       <c r="R20" s="23"/>
@@ -2599,16 +2596,16 @@
         <v>44</v>
       </c>
       <c r="F21" s="18">
-        <v>44985</v>
+        <v>45020</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="J21" s="20" t="s">
         <v>36</v>
@@ -2621,13 +2618,13 @@
         <v>36</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>218</v>
+        <v>162</v>
       </c>
       <c r="O21" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q21" s="20"/>
       <c r="R21" s="23"/>
@@ -2653,7 +2650,7 @@
         <v>45</v>
       </c>
       <c r="F22" s="18">
-        <v>44985</v>
+        <v>45021</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
@@ -2667,7 +2664,7 @@
       <c r="N22" s="20"/>
       <c r="O22" s="20"/>
       <c r="P22" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q22" s="20"/>
       <c r="R22" s="23"/>
@@ -2693,7 +2690,7 @@
         <v>45</v>
       </c>
       <c r="F23" s="18">
-        <v>44985</v>
+        <v>45020</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
@@ -2707,7 +2704,7 @@
       <c r="N23" s="20"/>
       <c r="O23" s="20"/>
       <c r="P23" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q23" s="20"/>
       <c r="R23" s="23"/>
@@ -2740,7 +2737,7 @@
         <v>124</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
@@ -2771,16 +2768,16 @@
         <v>51</v>
       </c>
       <c r="F25" s="18">
-        <v>44985</v>
+        <v>45021</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="H25" s="39" t="s">
-        <v>201</v>
+        <v>206</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>207</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="J25" s="20" t="s">
         <v>36</v>
@@ -2793,13 +2790,13 @@
         <v>36</v>
       </c>
       <c r="N25" s="20" t="s">
-        <v>206</v>
+        <v>161</v>
       </c>
       <c r="O25" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q25" s="20"/>
       <c r="R25" s="23"/>
@@ -2825,16 +2822,16 @@
         <v>53</v>
       </c>
       <c r="F26" s="18">
-        <v>44985</v>
+        <v>45021</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="J26" s="20" t="s">
         <v>36</v>
@@ -2847,13 +2844,13 @@
         <v>36</v>
       </c>
       <c r="N26" s="20" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="O26" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P26" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q26" s="20"/>
       <c r="R26" s="23"/>
@@ -2886,7 +2883,7 @@
         <v>124</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
@@ -2924,7 +2921,7 @@
         <v>124</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
@@ -2955,16 +2952,16 @@
         <v>59</v>
       </c>
       <c r="F29" s="18">
-        <v>44985</v>
+        <v>45021</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="J29" s="20" t="s">
         <v>36</v>
@@ -2977,13 +2974,13 @@
         <v>36</v>
       </c>
       <c r="N29" s="20" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="O29" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q29" s="20"/>
       <c r="R29" s="23"/>
@@ -2992,7 +2989,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="120.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <v>69</v>
       </c>
@@ -3009,16 +3006,16 @@
         <v>61</v>
       </c>
       <c r="F30" s="18">
-        <v>44985</v>
+        <v>45021</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>36</v>
@@ -3031,13 +3028,13 @@
         <v>36</v>
       </c>
       <c r="N30" s="20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O30" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P30" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q30" s="20"/>
       <c r="R30" s="23"/>
@@ -3070,7 +3067,7 @@
         <v>124</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
@@ -3108,7 +3105,7 @@
         <v>124</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>220</v>
+        <v>164</v>
       </c>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
@@ -3146,7 +3143,7 @@
         <v>124</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
@@ -3177,16 +3174,16 @@
         <v>69</v>
       </c>
       <c r="F34" s="18">
-        <v>44985</v>
+        <v>45021</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="J34" s="20" t="s">
         <v>36</v>
@@ -3199,13 +3196,13 @@
         <v>36</v>
       </c>
       <c r="N34" s="20" t="s">
-        <v>216</v>
+        <v>159</v>
       </c>
       <c r="O34" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P34" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q34" s="20"/>
       <c r="R34" s="23"/>
@@ -3238,7 +3235,7 @@
         <v>124</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
@@ -3276,7 +3273,7 @@
         <v>124</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
@@ -3307,16 +3304,16 @@
         <v>75</v>
       </c>
       <c r="F37" s="18">
-        <v>44978</v>
+        <v>45020</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="J37" s="20" t="s">
         <v>36</v>
@@ -3329,13 +3326,13 @@
         <v>36</v>
       </c>
       <c r="N37" s="20" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="O37" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P37" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q37" s="20"/>
       <c r="R37" s="23"/>
@@ -3361,16 +3358,16 @@
         <v>77</v>
       </c>
       <c r="F38" s="18">
-        <v>44978</v>
+        <v>45020</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="J38" s="20" t="s">
         <v>36</v>
@@ -3383,13 +3380,13 @@
         <v>36</v>
       </c>
       <c r="N38" s="20" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="O38" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P38" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q38" s="20"/>
       <c r="R38" s="23"/>
@@ -3422,7 +3419,7 @@
         <v>124</v>
       </c>
       <c r="K39" s="20" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="L39" s="20"/>
       <c r="M39" s="20"/>
@@ -3460,7 +3457,7 @@
         <v>124</v>
       </c>
       <c r="K40" s="20" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
@@ -3491,16 +3488,16 @@
         <v>83</v>
       </c>
       <c r="F41" s="18">
-        <v>44978</v>
+        <v>45020</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="I41" s="19" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="J41" s="20" t="s">
         <v>36</v>
@@ -3513,13 +3510,13 @@
         <v>36</v>
       </c>
       <c r="N41" s="20" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="O41" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q41" s="20"/>
       <c r="R41" s="23"/>
@@ -3552,7 +3549,7 @@
         <v>124</v>
       </c>
       <c r="K42" s="20" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="L42" s="20"/>
       <c r="M42" s="20"/>
@@ -3566,7 +3563,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <v>129</v>
       </c>
@@ -3583,16 +3580,16 @@
         <v>87</v>
       </c>
       <c r="F43" s="18">
-        <v>44978</v>
+        <v>45020</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="J43" s="20" t="s">
         <v>36</v>
@@ -3605,13 +3602,13 @@
         <v>36</v>
       </c>
       <c r="N43" s="20" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="O43" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P43" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q43" s="20"/>
       <c r="R43" s="23"/>
@@ -3644,7 +3641,7 @@
         <v>124</v>
       </c>
       <c r="K44" s="20" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="L44" s="20"/>
       <c r="M44" s="20"/>
@@ -3682,7 +3679,7 @@
         <v>124</v>
       </c>
       <c r="K45" s="20" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="L45" s="20"/>
       <c r="M45" s="20"/>
@@ -3720,7 +3717,7 @@
         <v>124</v>
       </c>
       <c r="K46" s="20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L46" s="20"/>
       <c r="M46" s="20"/>
@@ -3758,7 +3755,7 @@
         <v>124</v>
       </c>
       <c r="K47" s="20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L47" s="20"/>
       <c r="M47" s="20"/>
@@ -3796,7 +3793,7 @@
         <v>124</v>
       </c>
       <c r="K48" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L48" s="20"/>
       <c r="M48" s="20"/>
@@ -3834,7 +3831,7 @@
         <v>124</v>
       </c>
       <c r="K49" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L49" s="20"/>
       <c r="M49" s="20"/>
@@ -3872,7 +3869,7 @@
         <v>124</v>
       </c>
       <c r="K50" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L50" s="20"/>
       <c r="M50" s="20"/>
@@ -3910,7 +3907,7 @@
         <v>124</v>
       </c>
       <c r="K51" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L51" s="20"/>
       <c r="M51" s="20"/>
@@ -3948,7 +3945,7 @@
         <v>124</v>
       </c>
       <c r="K52" s="20" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="L52" s="20"/>
       <c r="M52" s="20"/>
@@ -3986,7 +3983,7 @@
         <v>124</v>
       </c>
       <c r="K53" s="20" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="L53" s="20"/>
       <c r="M53" s="20"/>
@@ -4017,16 +4014,16 @@
         <v>109</v>
       </c>
       <c r="F54" s="18">
-        <v>44978</v>
+        <v>45020</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="J54" s="20" t="s">
         <v>36</v>
@@ -4039,13 +4036,13 @@
         <v>36</v>
       </c>
       <c r="N54" s="20" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="O54" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P54" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q54" s="20"/>
       <c r="R54" s="23"/>
@@ -4078,7 +4075,7 @@
         <v>124</v>
       </c>
       <c r="K55" s="20" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="L55" s="20"/>
       <c r="M55" s="20"/>
@@ -4109,16 +4106,16 @@
         <v>113</v>
       </c>
       <c r="F56" s="18">
-        <v>44978</v>
+        <v>45020</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="J56" s="20" t="s">
         <v>36</v>
@@ -4131,13 +4128,13 @@
         <v>36</v>
       </c>
       <c r="N56" s="20" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="O56" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P56" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q56" s="20"/>
       <c r="R56" s="23"/>
@@ -4163,16 +4160,16 @@
         <v>115</v>
       </c>
       <c r="F57" s="18">
-        <v>44978</v>
+        <v>45020</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="J57" s="20" t="s">
         <v>36</v>
@@ -4185,13 +4182,13 @@
         <v>36</v>
       </c>
       <c r="N57" s="20" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="O57" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P57" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q57" s="20"/>
       <c r="R57" s="23"/>
@@ -4217,16 +4214,16 @@
         <v>117</v>
       </c>
       <c r="F58" s="18">
-        <v>44978</v>
+        <v>45020</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="H58" s="19" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="J58" s="20" t="s">
         <v>36</v>
@@ -4239,13 +4236,13 @@
         <v>36</v>
       </c>
       <c r="N58" s="20" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="O58" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P58" s="20" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="Q58" s="20"/>
       <c r="R58" s="23"/>
@@ -4278,7 +4275,7 @@
         <v>124</v>
       </c>
       <c r="K59" s="20" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="L59" s="20"/>
       <c r="M59" s="20"/>
@@ -4316,7 +4313,7 @@
         <v>124</v>
       </c>
       <c r="K60" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L60" s="20"/>
       <c r="M60" s="20"/>
@@ -19784,6 +19781,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -19792,7 +19800,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -20023,18 +20031,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -20042,7 +20056,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20061,23 +20075,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Riesecuzione dei test case in seguito a revisione del formato date e compilazione campi propedeutici per l'accreditamento.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
+++ b/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lavoro\FSE\Accreditamento\GitHub\GATEWAY\A1#111S3K00000000\S3K_SPA\JHIS\23.01.01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF9FACF-1812-4E56-A02F-6C11F1A03278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF17EA4-883C-4889-9B14-832861B6911D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="222">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -824,9 +824,6 @@
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>[Errore-47| codice fiscale 'ccrttc85t17l219' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]</t>
-  </si>
-  <si>
     <t>JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA</t>
   </si>
   <si>
@@ -839,187 +836,175 @@
     <t>Le installazioni di JHIS non prevedono la gestione della terapia farmacologica.</t>
   </si>
   <si>
-    <t>2023-04-04T15:14:17Z</t>
-  </si>
-  <si>
-    <t>7c5b99da8e7365d5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.ba58ea3e9ab92c9c9ec91e5b20038080ebc7bc87a778f9f02b1e83f1ae4905af.ce80a4b864^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e71701bb335f463f</t>
-  </si>
-  <si>
-    <t>2023-04-04T15:25:12Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.a98759b9cc4ecc1f11d04f219f1e89685c9b0a0872f6913561471fed8f1689fe.242cecf84f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>[ERRORE-47| codice fiscale 'ccrttc85t17l219' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]</t>
-  </si>
-  <si>
-    <t>2023-04-04T15:34:26Z</t>
-  </si>
-  <si>
-    <t>9b77a6781d233bf5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.ce9f51df2561b5a2741f052817a8f2ebeac210442c099db092fe9ac975fc9020.8dbbe9d9f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-04T15:38:28Z</t>
-  </si>
-  <si>
-    <t>46014514b8c70c4d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.1f19a337adb6950eaf924b4918849d2b2c1ef00ce044cb38b771a0536713ae03.cc6ae7089b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-04T15:47:29Z</t>
-  </si>
-  <si>
-    <t>f24b7c94b09caf54</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.2e45760309b813022c89ffccc9da99a5c10bc26bcc18ba12eaacd6539c82487a.a815e30e96^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'extension' on element 'id' is not valid with respect to its type, 'st'.,ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'extension' on element 'id' is not valid with respect to its type, 'st'.,ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'extension' on element 'id' is not valid with respect to its type, 'st'.</t>
   </si>
   <si>
-    <t>2023-04-04T16:02:39Z</t>
-  </si>
-  <si>
-    <t>67608899afc6146b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.56a1b2ea5a6acf1c61769c4bdd57f6747d89d605d8a28e1b6a7ac5060126f853.8732ba96ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-04T16:08:41Z</t>
-  </si>
-  <si>
-    <t>b23842c617353dbf</t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.54.1, Codes: X]</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.59233e4425c89d0dec3b5a70f35a7fefd6b18a73cea12bc0615b45e359577a7d.f1683f1aa4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.54.4, Codes: 0]</t>
   </si>
   <si>
-    <t>78c53bbd0b3e9dba</t>
-  </si>
-  <si>
-    <t>2023-04-04T16:14:46Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.9bf3394d7b9e190dd1ef5435bc3396007774e905cc77f8c11a17610e07ec9afc.22e752b624^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-04T16:26:27Z</t>
-  </si>
-  <si>
-    <t>07e80bdf413d9456</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.f8608eda5aec15c87b656123f6f984984e0cbd560585b3c9b30501609c0dbc14.36006402db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-04T16:30:46Z</t>
-  </si>
-  <si>
-    <t>778134e84e2f8763</t>
-  </si>
-  <si>
     <t>Messaggio fornito dal gateway (ad es. "Il campo person_id non è valorizzato")</t>
   </si>
   <si>
-    <t>a159dabd3d976444</t>
-  </si>
-  <si>
-    <t>2023-04-04T16:34:41Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.0885ca9bffa46c5fa7261baf51ae6d0916a0f39bc0f4dcaeb1733fec6a1066e7.1eba2a8230^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-05T14:48:27Z</t>
-  </si>
-  <si>
-    <t>c0b9d91dc6ca4795</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.76b382f83be34b865eb3028d8f5aad13d26a8eb035ebff5280139a7880b8be35.a7e281e348^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-05T14:55:25Z</t>
-  </si>
-  <si>
-    <t>b83202f3ed8a76fb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.a143c2a93d019639e260fc236d7a280711ec0270400543cf44b6febf5c8ee904.728a5535a7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-05T14:58:15Z</t>
-  </si>
-  <si>
-    <t>8fc4a9b043fa2026</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.68db232115c936bdd878925a9189086e1dded9efed4c7e5674421bb7beac7f87.c1c8a6b993^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-05T15:00:42Z</t>
-  </si>
-  <si>
-    <t>0fc62afe58458a49</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.315045872ba55a2f5523e9c634d536228d19442d71a7be3b7e4dffac123b934e.163ebb7186^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Errore semantico.","detail":"[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
   </si>
   <si>
-    <t>2023-04-05T15:03:00Z</t>
-  </si>
-  <si>
-    <t>5bf5d78d980db52a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.a0d10d08ef0ec59dfca253813cd836c6ad3402627c57dd6021dc21a682d94bc3.b0de6df423^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.2f5cd45674dd6509e79c475673691619c26e59fbe770a1d677fe10c9e0e79790.faaa4a8da9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5dd3a831a740715e</t>
-  </si>
-  <si>
-    <t>2023-04-05T15:05:18Z</t>
-  </si>
-  <si>
-    <t>2023-04-05T15:07:34Z</t>
-  </si>
-  <si>
-    <t>514732719f910c4e</t>
-  </si>
-  <si>
-    <t>2023-04-05T15:09:31Z</t>
-  </si>
-  <si>
-    <t>ff9fd12634e91e3a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.100.4.4.c877847a32eeaa6b8b1ecbf81bbd2d18b17c58098e7815b7dcb5450b05dba37e.7cfe857e71^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-05-22T11:53:03Z</t>
+  </si>
+  <si>
+    <t>1c531f7177ecba3a</t>
+  </si>
+  <si>
+    <t>2023-05-22T14:03:41Z</t>
+  </si>
+  <si>
+    <t>638a661d5d7440a3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.07ace36b3598504f4b65e18dff8ac6cf7720d7360505cf3f5bb0de1e8dde7c9e.25107746fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8b09c8681589f3e0</t>
+  </si>
+  <si>
+    <t>2023-05-22T14:19:44Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.20cc44b294cf5ec84510054ae19b1d19638cc60be7194d8fb582e258d5d6cdbf.e120c76606^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T14:23:58Z</t>
+  </si>
+  <si>
+    <t>61f2184eabfc7ebc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.d4a35a056ec307de09cc9e31a38df6adf903a5e9a3944b2ff5602757f370d2aa.ce5b6f97e7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T14:27:03Z</t>
+  </si>
+  <si>
+    <t>dea316d235e080c3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.2afd7c04b58ad16a9bc35e239f45197b81ef01df4f4b5029f4098b91e3e46976.701ee7af52^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T14:30:52Z</t>
+  </si>
+  <si>
+    <t>ade82183655bbf2f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.2a4def89ad5f31d2974c74101c580c513e061a42259c86301a545564f6d108ae.9cab19c897^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T14:34:09Z</t>
+  </si>
+  <si>
+    <t>0a9e34845f175bef</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.58e565a289f8f2ab3befd68d546c4a6930fa43e6481385ef11e6adce2e200042.804da14693^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T14:39:25Z</t>
+  </si>
+  <si>
+    <t>395c5ff96e0c5772</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.1b2c16f5281a582a07548a813ade9b81e94fb385304e2ad1bc8b6012c3373ec4.cd107db6c3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T14:42:43Z</t>
+  </si>
+  <si>
+    <t>d0cfc6f5811d41ef</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.cd9bfc3f0b0f2a61c69fc49857a50bef11240f91655134d3a5878d3457097737.a16ad7356c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T14:45:17Z</t>
+  </si>
+  <si>
+    <t>77378e044a0241a2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.8cbb24251f8963994b5695f351645b94bf047420515c5a18c9657a133a94fa3d.cae39444cc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T17:37:54Z</t>
+  </si>
+  <si>
+    <t>f8fefda252a7c225</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.3efa8575504a79078237043ce2a9d81883df89ec4986433f98d9e81e8aa3c891.3357f48568^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2806a2f0343d8c43</t>
+  </si>
+  <si>
+    <t>2023-05-22T17:45:42Z</t>
+  </si>
+  <si>
+    <t>2023-05-22T17:50:49Z</t>
+  </si>
+  <si>
+    <t>7c0ef420e8c7cb1e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.9938a5887e7553105498c06453da9b5c02a1865aed3091d35979893808c7e1d4.dbf67d53d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T17:55:24Z</t>
+  </si>
+  <si>
+    <t>14b0c2efaf8c9cfb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.7eab988145f3550be378290c42448bf7992a9a374f6cea4a9c23f2e0b3518bff.0495f2ecaa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T17:57:58Z</t>
+  </si>
+  <si>
+    <t>1cd68793e940f588</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.91c6b6c38edaf0354d95aeeabdbbc9b0795b6b1d624594ee7ddbbb07ab89d095.ad1de96c80^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T17:59:45Z</t>
+  </si>
+  <si>
+    <t>c0ce251cb85f14aa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.c31b18b2cb9a26ba2bd52a6210d5ab401633a30a30541ef5069edfe80b962ba1.87fe0acba8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-22T18:01:19Z</t>
+  </si>
+  <si>
+    <t>33dec415993c1139</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.7a2956771753b77fa25a9adc6b363f5369f18f2a4ee50eb78c0e8e67120e3e6d.63c72b4dba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>91249f79c6f81aee</t>
+  </si>
+  <si>
+    <t>2023-05-22T18:04:56Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.100.4.4.7c008757e01f3bc20606d56e2e044e0223025ba5c3b26ff6238a079622f1af4f.7f977d1ee9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1837,10 +1822,10 @@
   <dimension ref="A1:T905"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,16 +2103,16 @@
         <v>20</v>
       </c>
       <c r="F10" s="18">
-        <v>45021</v>
+        <v>45068</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J10" s="20" t="s">
         <v>36</v>
@@ -2275,22 +2260,16 @@
       <c r="E14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="18">
-        <v>45020</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>168</v>
-      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
       <c r="J14" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="20"/>
+        <v>124</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>146</v>
+      </c>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
@@ -2434,13 +2413,13 @@
         <v>38</v>
       </c>
       <c r="F18" s="18">
-        <v>45021</v>
+        <v>45068</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="I18" s="19" t="s">
         <v>160</v>
@@ -2456,13 +2435,13 @@
         <v>36</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="O18" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P18" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q18" s="20"/>
       <c r="R18" s="23"/>
@@ -2488,13 +2467,13 @@
         <v>40</v>
       </c>
       <c r="F19" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="I19" s="19" t="s">
         <v>160</v>
@@ -2510,13 +2489,13 @@
         <v>36</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="O19" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P19" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q19" s="20"/>
       <c r="R19" s="23"/>
@@ -2542,16 +2521,16 @@
         <v>42</v>
       </c>
       <c r="F20" s="18">
-        <v>45021</v>
+        <v>45068</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="J20" s="20" t="s">
         <v>36</v>
@@ -2564,13 +2543,13 @@
         <v>36</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O20" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P20" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q20" s="20"/>
       <c r="R20" s="23"/>
@@ -2596,16 +2575,16 @@
         <v>44</v>
       </c>
       <c r="F21" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="J21" s="20" t="s">
         <v>36</v>
@@ -2618,13 +2597,13 @@
         <v>36</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O21" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q21" s="20"/>
       <c r="R21" s="23"/>
@@ -2650,7 +2629,7 @@
         <v>45</v>
       </c>
       <c r="F22" s="18">
-        <v>45021</v>
+        <v>45068</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
@@ -2664,7 +2643,7 @@
       <c r="N22" s="20"/>
       <c r="O22" s="20"/>
       <c r="P22" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q22" s="20"/>
       <c r="R22" s="23"/>
@@ -2690,7 +2669,7 @@
         <v>45</v>
       </c>
       <c r="F23" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
@@ -2704,7 +2683,7 @@
       <c r="N23" s="20"/>
       <c r="O23" s="20"/>
       <c r="P23" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q23" s="20"/>
       <c r="R23" s="23"/>
@@ -2768,16 +2747,16 @@
         <v>51</v>
       </c>
       <c r="F25" s="18">
-        <v>45021</v>
+        <v>45068</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J25" s="20" t="s">
         <v>36</v>
@@ -2796,7 +2775,7 @@
         <v>124</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q25" s="20"/>
       <c r="R25" s="23"/>
@@ -2822,16 +2801,16 @@
         <v>53</v>
       </c>
       <c r="F26" s="18">
-        <v>45021</v>
+        <v>45068</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="J26" s="20" t="s">
         <v>36</v>
@@ -2850,7 +2829,7 @@
         <v>124</v>
       </c>
       <c r="P26" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q26" s="20"/>
       <c r="R26" s="23"/>
@@ -2952,16 +2931,16 @@
         <v>59</v>
       </c>
       <c r="F29" s="18">
-        <v>45021</v>
+        <v>45068</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J29" s="20" t="s">
         <v>36</v>
@@ -2980,7 +2959,7 @@
         <v>124</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q29" s="20"/>
       <c r="R29" s="23"/>
@@ -3006,7 +2985,7 @@
         <v>61</v>
       </c>
       <c r="F30" s="18">
-        <v>45021</v>
+        <v>45068</v>
       </c>
       <c r="G30" s="19" t="s">
         <v>216</v>
@@ -3028,13 +3007,13 @@
         <v>36</v>
       </c>
       <c r="N30" s="20" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="O30" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P30" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q30" s="20"/>
       <c r="R30" s="23"/>
@@ -3105,7 +3084,7 @@
         <v>124</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
@@ -3143,7 +3122,7 @@
         <v>124</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
@@ -3174,16 +3153,16 @@
         <v>69</v>
       </c>
       <c r="F34" s="18">
-        <v>45021</v>
+        <v>45068</v>
       </c>
       <c r="G34" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="I34" s="19" t="s">
         <v>221</v>
-      </c>
-      <c r="H34" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="I34" s="19" t="s">
-        <v>219</v>
       </c>
       <c r="J34" s="20" t="s">
         <v>36</v>
@@ -3202,7 +3181,7 @@
         <v>124</v>
       </c>
       <c r="P34" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q34" s="20"/>
       <c r="R34" s="23"/>
@@ -3235,7 +3214,7 @@
         <v>124</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
@@ -3287,7 +3266,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="120.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>123</v>
       </c>
@@ -3304,16 +3283,16 @@
         <v>75</v>
       </c>
       <c r="F37" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="J37" s="20" t="s">
         <v>36</v>
@@ -3326,13 +3305,13 @@
         <v>36</v>
       </c>
       <c r="N37" s="20" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="O37" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P37" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q37" s="20"/>
       <c r="R37" s="23"/>
@@ -3341,7 +3320,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <v>124</v>
       </c>
@@ -3358,16 +3337,16 @@
         <v>77</v>
       </c>
       <c r="F38" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="J38" s="20" t="s">
         <v>36</v>
@@ -3386,7 +3365,7 @@
         <v>124</v>
       </c>
       <c r="P38" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q38" s="20"/>
       <c r="R38" s="23"/>
@@ -3488,16 +3467,16 @@
         <v>83</v>
       </c>
       <c r="F41" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="I41" s="19" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="J41" s="20" t="s">
         <v>36</v>
@@ -3516,7 +3495,7 @@
         <v>124</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q41" s="20"/>
       <c r="R41" s="23"/>
@@ -3580,16 +3559,16 @@
         <v>87</v>
       </c>
       <c r="F43" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="J43" s="20" t="s">
         <v>36</v>
@@ -3602,13 +3581,13 @@
         <v>36</v>
       </c>
       <c r="N43" s="20" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="O43" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P43" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q43" s="20"/>
       <c r="R43" s="23"/>
@@ -4014,16 +3993,16 @@
         <v>109</v>
       </c>
       <c r="F54" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="J54" s="20" t="s">
         <v>36</v>
@@ -4042,7 +4021,7 @@
         <v>124</v>
       </c>
       <c r="P54" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q54" s="20"/>
       <c r="R54" s="23"/>
@@ -4075,7 +4054,7 @@
         <v>124</v>
       </c>
       <c r="K55" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L55" s="20"/>
       <c r="M55" s="20"/>
@@ -4106,16 +4085,16 @@
         <v>113</v>
       </c>
       <c r="F56" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="J56" s="20" t="s">
         <v>36</v>
@@ -4128,13 +4107,13 @@
         <v>36</v>
       </c>
       <c r="N56" s="20" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="O56" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P56" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q56" s="20"/>
       <c r="R56" s="23"/>
@@ -4160,16 +4139,16 @@
         <v>115</v>
       </c>
       <c r="F57" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J57" s="20" t="s">
         <v>36</v>
@@ -4182,13 +4161,13 @@
         <v>36</v>
       </c>
       <c r="N57" s="20" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="O57" s="20" t="s">
         <v>124</v>
       </c>
       <c r="P57" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q57" s="20"/>
       <c r="R57" s="23"/>
@@ -4214,16 +4193,16 @@
         <v>117</v>
       </c>
       <c r="F58" s="18">
-        <v>45020</v>
+        <v>45068</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H58" s="19" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J58" s="20" t="s">
         <v>36</v>
@@ -4242,7 +4221,7 @@
         <v>124</v>
       </c>
       <c r="P58" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q58" s="20"/>
       <c r="R58" s="23"/>
@@ -4275,7 +4254,7 @@
         <v>124</v>
       </c>
       <c r="K59" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L59" s="20"/>
       <c r="M59" s="20"/>
@@ -18704,8 +18683,8 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -19781,26 +19760,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -20031,32 +19990,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20075,6 +20029,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Dettagliata gestione degli errori.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
+++ b/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lavoro\FSE\Accreditamento\GitHub\GATEWAY\A1#111S3K00000000\S3K_SPA\JHIS\23.01.01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF17EA4-883C-4889-9B14-832861B6911D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2314597-FFFF-4870-90C1-4BDB52B3AEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="225">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -1005,6 +1005,26 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.100.4.4.7c008757e01f3bc20606d56e2e044e0223025ba5c3b26ff6238a079622f1af4f.7f977d1ee9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>La validazione può avvenire in due momenti differenti:
+1. alla generazione del documento
+2. prima della firma del documento
+Il secondo caso potrebbe quindi sanare eventuali anomalie di timeout occorse durante il primo tentativo.
+In caso di insuccesso di entrambi i tentativi, il documento verrà validato via batch da un processo schedulato.</t>
+  </si>
+  <si>
+    <t>Assunto: la nostra soluzione cerca di limitare l'inserimento manuale delle informazioni che richiedono una codifica, pertanto l'utente è guidato nella selezione dei valori e successivamente, prima di essere salvati ed inseriti nel CDA, vengono validati.
+A seconda della tipologia di dato mancante, si procederà alla verifica e correzione delle informazioni.
+Ad es.:
+ - in presenza di codice fiscale paziente formalmente errato, si chiederà agli operatori di correggere l'anagrafica
+ - in presenza di utente sprovvisto di codice fiscale, il supporto procederà con l'arricchimento dell'anagrafica utente
+In caso di errore non recuperabile, il documento verrà rigenerato con le informazioni aggiornate e reinviato al processo di validazione</t>
+  </si>
+  <si>
+    <t>Assunto: la nostra soluzione cerca di limitare l'inserimento manuale delle informazioni che richiedono una codifica, pertanto l'utente è guidato nella selezione dei valori e successivamente, prima di essere salvati ed inseriti nel CDA, vengono validati.
+La transcodifica delle informazioni è gestita internamente dal sistema di generazione del CDA tramite apposite tabelle, pertanto le anomalie ad essa riconducibili sono limitate ad un dominio ristretto di informazioni.
+In ogni caso, eventuali anomalie monitorate da un processo batch verranno inoltrate ad un gruppo di lavoro che si occuperà di correggere i dati e procedere nuovamente alla rigenerazione e validazione del documento.</t>
   </si>
 </sst>
 </file>
@@ -1822,10 +1842,10 @@
   <dimension ref="A1:T905"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,7 +2416,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>29</v>
       </c>
@@ -2438,10 +2458,10 @@
         <v>168</v>
       </c>
       <c r="O18" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P18" s="20" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="Q18" s="20"/>
       <c r="R18" s="23"/>
@@ -2450,7 +2470,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>35</v>
       </c>
@@ -2492,10 +2512,10 @@
         <v>168</v>
       </c>
       <c r="O19" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P19" s="20" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="Q19" s="20"/>
       <c r="R19" s="23"/>
@@ -2504,7 +2524,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>37</v>
       </c>
@@ -2546,10 +2566,10 @@
         <v>161</v>
       </c>
       <c r="O20" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P20" s="20" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="Q20" s="20"/>
       <c r="R20" s="23"/>
@@ -2558,7 +2578,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>43</v>
       </c>
@@ -2600,10 +2620,10 @@
         <v>161</v>
       </c>
       <c r="O21" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="Q21" s="20"/>
       <c r="R21" s="23"/>
@@ -2612,7 +2632,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>45</v>
       </c>
@@ -2643,7 +2663,7 @@
       <c r="N22" s="20"/>
       <c r="O22" s="20"/>
       <c r="P22" s="20" t="s">
-        <v>162</v>
+        <v>222</v>
       </c>
       <c r="Q22" s="20"/>
       <c r="R22" s="23"/>
@@ -2652,7 +2672,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>51</v>
       </c>
@@ -2683,7 +2703,7 @@
       <c r="N23" s="20"/>
       <c r="O23" s="20"/>
       <c r="P23" s="20" t="s">
-        <v>162</v>
+        <v>222</v>
       </c>
       <c r="Q23" s="20"/>
       <c r="R23" s="23"/>
@@ -2784,7 +2804,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>65</v>
       </c>
@@ -2829,7 +2849,7 @@
         <v>124</v>
       </c>
       <c r="P26" s="20" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="Q26" s="20"/>
       <c r="R26" s="23"/>
@@ -2838,7 +2858,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="120.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <v>66</v>
       </c>
@@ -2914,7 +2934,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <v>68</v>
       </c>
@@ -2956,10 +2976,10 @@
         <v>152</v>
       </c>
       <c r="O29" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="Q29" s="20"/>
       <c r="R29" s="23"/>
@@ -3136,7 +3156,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>73</v>
       </c>
@@ -3178,10 +3198,10 @@
         <v>159</v>
       </c>
       <c r="O34" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P34" s="20" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="Q34" s="20"/>
       <c r="R34" s="23"/>
@@ -3365,7 +3385,7 @@
         <v>124</v>
       </c>
       <c r="P38" s="20" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="Q38" s="20"/>
       <c r="R38" s="23"/>
@@ -3450,7 +3470,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
         <v>127</v>
       </c>
@@ -3492,10 +3512,10 @@
         <v>152</v>
       </c>
       <c r="O41" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="Q41" s="20"/>
       <c r="R41" s="23"/>
@@ -4068,7 +4088,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <v>142</v>
       </c>
@@ -4110,10 +4130,10 @@
         <v>166</v>
       </c>
       <c r="O56" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P56" s="20" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="Q56" s="20"/>
       <c r="R56" s="23"/>
@@ -4122,7 +4142,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="15">
         <v>143</v>
       </c>
@@ -4164,10 +4184,10 @@
         <v>167</v>
       </c>
       <c r="O57" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P57" s="20" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="Q57" s="20"/>
       <c r="R57" s="23"/>
@@ -4218,10 +4238,10 @@
         <v>159</v>
       </c>
       <c r="O58" s="20" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="P58" s="20" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="Q58" s="20"/>
       <c r="R58" s="23"/>
@@ -18692,7 +18712,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O1:O8 L1:M8 O10:O1048576 L10:M1048576</xm:sqref>
+          <xm:sqref>O1:O8 L1:M8 L10:M1048576 O10:O1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
@@ -19760,6 +19780,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -19990,27 +20030,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20029,31 +20074,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Dettagliata gestione degli errori in seguito a mail del 31/05.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
+++ b/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lavoro\FSE\Accreditamento\GitHub\GATEWAY\A1#111S3K00000000\S3K_SPA\JHIS\23.01.01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2314597-FFFF-4870-90C1-4BDB52B3AEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629AFDD8-B6B2-4F52-88E2-80C1C8AA1567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1015,16 +1015,11 @@
   </si>
   <si>
     <t>Assunto: la nostra soluzione cerca di limitare l'inserimento manuale delle informazioni che richiedono una codifica, pertanto l'utente è guidato nella selezione dei valori e successivamente, prima di essere salvati ed inseriti nel CDA, vengono validati.
-A seconda della tipologia di dato mancante, si procederà alla verifica e correzione delle informazioni.
-Ad es.:
- - in presenza di codice fiscale paziente formalmente errato, si chiederà agli operatori di correggere l'anagrafica
- - in presenza di utente sprovvisto di codice fiscale, il supporto procederà con l'arricchimento dell'anagrafica utente
-In caso di errore non recuperabile, il documento verrà rigenerato con le informazioni aggiornate e reinviato al processo di validazione</t>
-  </si>
-  <si>
-    <t>Assunto: la nostra soluzione cerca di limitare l'inserimento manuale delle informazioni che richiedono una codifica, pertanto l'utente è guidato nella selezione dei valori e successivamente, prima di essere salvati ed inseriti nel CDA, vengono validati.
 La transcodifica delle informazioni è gestita internamente dal sistema di generazione del CDA tramite apposite tabelle, pertanto le anomalie ad essa riconducibili sono limitate ad un dominio ristretto di informazioni.
 In ogni caso, eventuali anomalie monitorate da un processo batch verranno inoltrate ad un gruppo di lavoro che si occuperà di correggere i dati e procedere nuovamente alla rigenerazione e validazione del documento.</t>
+  </si>
+  <si>
+    <t>Si procede con l'analisi dell'errore ad alla sua correzione.</t>
   </si>
 </sst>
 </file>
@@ -1845,7 +1840,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2416,7 +2411,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>29</v>
       </c>
@@ -2461,7 +2456,7 @@
         <v>36</v>
       </c>
       <c r="P18" s="20" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Q18" s="20"/>
       <c r="R18" s="23"/>
@@ -2470,7 +2465,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>35</v>
       </c>
@@ -2515,7 +2510,7 @@
         <v>36</v>
       </c>
       <c r="P19" s="20" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Q19" s="20"/>
       <c r="R19" s="23"/>
@@ -2524,7 +2519,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>37</v>
       </c>
@@ -2569,7 +2564,7 @@
         <v>36</v>
       </c>
       <c r="P20" s="20" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Q20" s="20"/>
       <c r="R20" s="23"/>
@@ -2578,7 +2573,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>43</v>
       </c>
@@ -2623,7 +2618,7 @@
         <v>36</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Q21" s="20"/>
       <c r="R21" s="23"/>
@@ -2849,7 +2844,7 @@
         <v>124</v>
       </c>
       <c r="P26" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q26" s="20"/>
       <c r="R26" s="23"/>
@@ -2979,7 +2974,7 @@
         <v>36</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q29" s="20"/>
       <c r="R29" s="23"/>
@@ -3201,7 +3196,7 @@
         <v>36</v>
       </c>
       <c r="P34" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q34" s="20"/>
       <c r="R34" s="23"/>
@@ -3385,7 +3380,7 @@
         <v>124</v>
       </c>
       <c r="P38" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q38" s="20"/>
       <c r="R38" s="23"/>
@@ -3515,7 +3510,7 @@
         <v>36</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q41" s="20"/>
       <c r="R41" s="23"/>
@@ -4133,7 +4128,7 @@
         <v>36</v>
       </c>
       <c r="P56" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q56" s="20"/>
       <c r="R56" s="23"/>
@@ -4187,7 +4182,7 @@
         <v>36</v>
       </c>
       <c r="P57" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q57" s="20"/>
       <c r="R57" s="23"/>
@@ -4241,7 +4236,7 @@
         <v>36</v>
       </c>
       <c r="P58" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q58" s="20"/>
       <c r="R58" s="23"/>
@@ -19780,26 +19775,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -20030,32 +20005,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20074,6 +20044,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Esecuzione dei test case per 'RefertoSpecialisticaAmbulatoriale' propedeutici all'accreditamento.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
+++ b/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lavoro\FSE\Accreditamento\GitHub\GATEWAY\A1#111S3K00000000\S3K_SPA\JHIS\23.01.01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lavoro\FSE\Accreditamento\GitHub\GATEWAY\A1#111S3K00000000\S3K_SPA\JHIS\23.01.01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629AFDD8-B6B2-4F52-88E2-80C1C8AA1567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005E25C9-22C4-443E-8863-6047831E6DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="4" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$9:$T$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$9:$T$87</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="300">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -1021,12 +1021,369 @@
   <si>
     <t>Si procede con l'analisi dell'errore ad alla sua correzione.</t>
   </si>
+  <si>
+    <t>RSA</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_RSA_KO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Precondizioni:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Il fornitore utilizza un token jwt mancante di campi obbligatori, quindi non valido.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Descrizione di Business del caso di test: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Al fine di rendere non valido il token è necessario non valorizzare nel JWT il campo "purpose_of_use".</t>
+    </r>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Precondizioni:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Il fornitore utilizza un token jwt con dei campi valorizzati in maniera errata.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Descrizione di Business del caso di test: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt avente dei campi valorizzati in maniera errata al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Al fine di rendere non valido il token è necessario valorizzare il campo "action_id" con la stringa "TEST" (valore non ammesso).</t>
+    </r>
+  </si>
+  <si>
+    <t>VALIDAZIONE_RSA_TIMEOUT</t>
+  </si>
+  <si>
+    <t>Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nelle colonne relative a:
+"ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", "GESTIONE ERRORE".</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT6_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT7_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT8_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT9_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT10_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT11_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT15_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT16_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT17_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT18_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT19_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT20_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT21_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT22_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT23_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>2023-11-23T10:12:54Z</t>
+  </si>
+  <si>
+    <t>d0bdffe2d10f00e5</t>
+  </si>
+  <si>
+    <t>Messaggio fornito dal gateway (ad es. "Il campo purpose_of_use non è valorizzato")</t>
+  </si>
+  <si>
+    <t>2023-11-23T10:24:26Z</t>
+  </si>
+  <si>
+    <t>53cb041e27fd5523</t>
+  </si>
+  <si>
+    <t>Il campo action_id non è corretto</t>
+  </si>
+  <si>
+    <t>2023-11-23T10:29:34Z</t>
+  </si>
+  <si>
+    <t>ef736e57722d03ee</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.645e150ee82d85810fe377e6a8c90d2d99c9949b51959a92401be76bf30f0fbe.4af9b699da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-23T11:32:08Z</t>
+  </si>
+  <si>
+    <t>18901f79e59e6b67</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.e09aa0b3cb0fbc2e978eab74e8d5c136a4102982ac0d9b7dd98a1d8b4cc5285b.f8fb34dfeb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-44| Il codice fiscale 'ccrttc85t17l219o' cittadino ed operatore deve essere costituito da 16 cifre [A-Z0-9]{16}]</t>
+  </si>
+  <si>
+    <t>2023-11-23T11:36:24Z</t>
+  </si>
+  <si>
+    <t>d37b69c150f38037</t>
+  </si>
+  <si>
+    <t>[ERRORE-6| L'elemento ClinicalDocument/confidentialityCode DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25'</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.f1b8a272ed55eeada47c1d9b195bd466d86cda45e83c8662a41292981c5bb2f9.574aef3de5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il sesso del paziente è sempre obbligatorio. Inoltre, la conversione in XML verifica la presenza dei campi contrassegnati come obbligatori.</t>
+  </si>
+  <si>
+    <t>Il documento è sempre firmato manualmente o digitalmente.</t>
+  </si>
+  <si>
+    <t>Impossibile contattare l'FSE"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="13" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1114,6 +1471,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1329,7 +1698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1422,6 +1791,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1462,6 +1858,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1886,14 +2285,14 @@
       <c r="T1" s="8"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="31"/>
+      <c r="D2" s="40"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1911,14 +2310,14 @@
       <c r="T2" s="8"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="40"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -1936,12 +2335,12 @@
       <c r="T3" s="8"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="39" t="s">
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="10"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1960,12 +2359,12 @@
       <c r="T4" s="8"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="39" t="s">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="40"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -1983,8 +2382,8 @@
       <c r="T5" s="8"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="11"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4283,7 +4682,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15">
         <v>146</v>
       </c>
@@ -4321,466 +4720,1113 @@
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="8"/>
-      <c r="M61" s="8"/>
-      <c r="N61" s="8"/>
-      <c r="O61" s="8"/>
-      <c r="P61" s="8"/>
-      <c r="Q61" s="8"/>
-      <c r="R61" s="22"/>
-      <c r="S61" s="9"/>
-      <c r="T61" s="8"/>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="8"/>
-      <c r="M62" s="8"/>
-      <c r="N62" s="8"/>
-      <c r="O62" s="8"/>
-      <c r="P62" s="8"/>
-      <c r="Q62" s="8"/>
-      <c r="R62" s="22"/>
-      <c r="S62" s="9"/>
-      <c r="T62" s="8"/>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="8"/>
-      <c r="M63" s="8"/>
-      <c r="N63" s="8"/>
-      <c r="O63" s="8"/>
-      <c r="P63" s="8"/>
-      <c r="Q63" s="8"/>
-      <c r="R63" s="22"/>
-      <c r="S63" s="9"/>
-      <c r="T63" s="8"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
-      <c r="I64" s="7"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="8"/>
-      <c r="L64" s="8"/>
-      <c r="M64" s="8"/>
-      <c r="N64" s="8"/>
-      <c r="O64" s="8"/>
-      <c r="P64" s="8"/>
-      <c r="Q64" s="8"/>
-      <c r="R64" s="22"/>
-      <c r="S64" s="9"/>
-      <c r="T64" s="8"/>
-    </row>
-    <row r="65" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-      <c r="I65" s="7"/>
-      <c r="J65" s="8"/>
-      <c r="K65" s="8"/>
-      <c r="L65" s="8"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="8"/>
-      <c r="O65" s="8"/>
-      <c r="P65" s="8"/>
-      <c r="Q65" s="8"/>
-      <c r="R65" s="22"/>
-      <c r="S65" s="9"/>
-      <c r="T65" s="8"/>
-    </row>
-    <row r="66" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="8"/>
-      <c r="M66" s="8"/>
-      <c r="N66" s="8"/>
-      <c r="O66" s="8"/>
-      <c r="P66" s="8"/>
-      <c r="Q66" s="8"/>
-      <c r="R66" s="22"/>
-      <c r="S66" s="9"/>
-      <c r="T66" s="8"/>
-    </row>
-    <row r="67" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="I67" s="7"/>
-      <c r="J67" s="8"/>
-      <c r="K67" s="8"/>
-      <c r="L67" s="8"/>
-      <c r="M67" s="8"/>
-      <c r="N67" s="8"/>
-      <c r="O67" s="8"/>
-      <c r="P67" s="8"/>
-      <c r="Q67" s="8"/>
-      <c r="R67" s="22"/>
-      <c r="S67" s="9"/>
-      <c r="T67" s="8"/>
-    </row>
-    <row r="68" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-      <c r="L68" s="8"/>
-      <c r="M68" s="8"/>
-      <c r="N68" s="8"/>
-      <c r="O68" s="8"/>
-      <c r="P68" s="8"/>
-      <c r="Q68" s="8"/>
-      <c r="R68" s="22"/>
-      <c r="S68" s="9"/>
-      <c r="T68" s="8"/>
-    </row>
-    <row r="69" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-      <c r="I69" s="7"/>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-      <c r="L69" s="8"/>
-      <c r="M69" s="8"/>
-      <c r="N69" s="8"/>
-      <c r="O69" s="8"/>
-      <c r="P69" s="8"/>
-      <c r="Q69" s="8"/>
-      <c r="R69" s="22"/>
-      <c r="S69" s="9"/>
-      <c r="T69" s="8"/>
-    </row>
-    <row r="70" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="8"/>
-      <c r="M70" s="8"/>
-      <c r="N70" s="8"/>
-      <c r="O70" s="8"/>
-      <c r="P70" s="8"/>
-      <c r="Q70" s="8"/>
-      <c r="R70" s="22"/>
-      <c r="S70" s="9"/>
-      <c r="T70" s="8"/>
-    </row>
-    <row r="71" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8"/>
-      <c r="L71" s="8"/>
-      <c r="M71" s="8"/>
-      <c r="N71" s="8"/>
-      <c r="O71" s="8"/>
-      <c r="P71" s="8"/>
-      <c r="Q71" s="8"/>
-      <c r="R71" s="22"/>
-      <c r="S71" s="9"/>
-      <c r="T71" s="8"/>
-    </row>
-    <row r="72" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-      <c r="I72" s="7"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="8"/>
-      <c r="L72" s="8"/>
-      <c r="M72" s="8"/>
-      <c r="N72" s="8"/>
-      <c r="O72" s="8"/>
-      <c r="P72" s="8"/>
-      <c r="Q72" s="8"/>
-      <c r="R72" s="22"/>
-      <c r="S72" s="9"/>
-      <c r="T72" s="8"/>
-    </row>
-    <row r="73" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="8"/>
-      <c r="K73" s="8"/>
-      <c r="L73" s="8"/>
-      <c r="M73" s="8"/>
-      <c r="N73" s="8"/>
-      <c r="O73" s="8"/>
-      <c r="P73" s="8"/>
-      <c r="Q73" s="8"/>
-      <c r="R73" s="22"/>
-      <c r="S73" s="9"/>
-      <c r="T73" s="8"/>
-    </row>
-    <row r="74" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="7"/>
-      <c r="I74" s="7"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="8"/>
-      <c r="M74" s="8"/>
-      <c r="N74" s="8"/>
-      <c r="O74" s="8"/>
-      <c r="P74" s="8"/>
-      <c r="Q74" s="8"/>
-      <c r="R74" s="22"/>
-      <c r="S74" s="9"/>
-      <c r="T74" s="8"/>
-    </row>
-    <row r="75" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="I75" s="7"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="8"/>
-      <c r="L75" s="8"/>
-      <c r="M75" s="8"/>
-      <c r="N75" s="8"/>
-      <c r="O75" s="8"/>
-      <c r="P75" s="8"/>
-      <c r="Q75" s="8"/>
-      <c r="R75" s="22"/>
-      <c r="S75" s="9"/>
-      <c r="T75" s="8"/>
-    </row>
-    <row r="76" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-      <c r="H76" s="7"/>
-      <c r="I76" s="7"/>
-      <c r="J76" s="8"/>
-      <c r="K76" s="8"/>
-      <c r="L76" s="8"/>
-      <c r="M76" s="8"/>
-      <c r="N76" s="8"/>
-      <c r="O76" s="8"/>
-      <c r="P76" s="8"/>
-      <c r="Q76" s="8"/>
-      <c r="R76" s="22"/>
-      <c r="S76" s="9"/>
-      <c r="T76" s="8"/>
-    </row>
-    <row r="77" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="7"/>
-      <c r="I77" s="7"/>
-      <c r="J77" s="8"/>
-      <c r="K77" s="8"/>
-      <c r="L77" s="8"/>
-      <c r="M77" s="8"/>
-      <c r="N77" s="8"/>
-      <c r="O77" s="8"/>
-      <c r="P77" s="8"/>
-      <c r="Q77" s="8"/>
-      <c r="R77" s="22"/>
-      <c r="S77" s="9"/>
-      <c r="T77" s="8"/>
-    </row>
-    <row r="78" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
-      <c r="I78" s="7"/>
-      <c r="J78" s="8"/>
-      <c r="K78" s="8"/>
-      <c r="L78" s="8"/>
-      <c r="M78" s="8"/>
-      <c r="N78" s="8"/>
-      <c r="O78" s="8"/>
-      <c r="P78" s="8"/>
-      <c r="Q78" s="8"/>
-      <c r="R78" s="22"/>
-      <c r="S78" s="9"/>
-      <c r="T78" s="8"/>
-    </row>
-    <row r="79" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-      <c r="I79" s="7"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="8"/>
-      <c r="L79" s="8"/>
-      <c r="M79" s="8"/>
-      <c r="N79" s="8"/>
-      <c r="O79" s="8"/>
-      <c r="P79" s="8"/>
-      <c r="Q79" s="8"/>
-      <c r="R79" s="22"/>
-      <c r="S79" s="9"/>
-      <c r="T79" s="8"/>
-    </row>
-    <row r="80" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F80" s="7"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="7"/>
-      <c r="I80" s="7"/>
-      <c r="J80" s="8"/>
-      <c r="K80" s="8"/>
-      <c r="L80" s="8"/>
-      <c r="M80" s="8"/>
-      <c r="N80" s="8"/>
-      <c r="O80" s="8"/>
-      <c r="P80" s="8"/>
-      <c r="Q80" s="8"/>
-      <c r="R80" s="22"/>
-      <c r="S80" s="9"/>
-      <c r="T80" s="8"/>
-    </row>
-    <row r="81" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-      <c r="H81" s="7"/>
-      <c r="I81" s="7"/>
-      <c r="J81" s="8"/>
-      <c r="K81" s="8"/>
-      <c r="L81" s="8"/>
-      <c r="M81" s="8"/>
-      <c r="N81" s="8"/>
-      <c r="O81" s="8"/>
-      <c r="P81" s="8"/>
-      <c r="Q81" s="8"/>
-      <c r="R81" s="22"/>
-      <c r="S81" s="9"/>
-      <c r="T81" s="8"/>
-    </row>
-    <row r="82" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
-      <c r="H82" s="7"/>
-      <c r="I82" s="7"/>
-      <c r="J82" s="8"/>
-      <c r="K82" s="8"/>
-      <c r="L82" s="8"/>
-      <c r="M82" s="8"/>
-      <c r="N82" s="8"/>
-      <c r="O82" s="8"/>
-      <c r="P82" s="8"/>
-      <c r="Q82" s="8"/>
-      <c r="R82" s="22"/>
-      <c r="S82" s="9"/>
-      <c r="T82" s="8"/>
-    </row>
-    <row r="83" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F83" s="7"/>
-      <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
-      <c r="I83" s="7"/>
-      <c r="J83" s="8"/>
-      <c r="K83" s="8"/>
-      <c r="L83" s="8"/>
-      <c r="M83" s="8"/>
-      <c r="N83" s="8"/>
-      <c r="O83" s="8"/>
-      <c r="P83" s="8"/>
-      <c r="Q83" s="8"/>
-      <c r="R83" s="22"/>
-      <c r="S83" s="9"/>
-      <c r="T83" s="8"/>
-    </row>
-    <row r="84" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F84" s="7"/>
-      <c r="G84" s="7"/>
-      <c r="H84" s="7"/>
-      <c r="I84" s="7"/>
-      <c r="J84" s="8"/>
-      <c r="K84" s="8"/>
-      <c r="L84" s="8"/>
-      <c r="M84" s="8"/>
-      <c r="N84" s="8"/>
-      <c r="O84" s="8"/>
-      <c r="P84" s="8"/>
-      <c r="Q84" s="8"/>
-      <c r="R84" s="22"/>
-      <c r="S84" s="9"/>
-      <c r="T84" s="8"/>
-    </row>
-    <row r="85" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F85" s="7"/>
-      <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
-      <c r="I85" s="7"/>
-      <c r="J85" s="8"/>
-      <c r="K85" s="8"/>
-      <c r="L85" s="8"/>
-      <c r="M85" s="8"/>
-      <c r="N85" s="8"/>
-      <c r="O85" s="8"/>
-      <c r="P85" s="8"/>
-      <c r="Q85" s="8"/>
-      <c r="R85" s="22"/>
-      <c r="S85" s="9"/>
-      <c r="T85" s="8"/>
-    </row>
-    <row r="86" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-      <c r="I86" s="7"/>
-      <c r="J86" s="8"/>
-      <c r="K86" s="8"/>
-      <c r="L86" s="8"/>
-      <c r="M86" s="8"/>
-      <c r="N86" s="8"/>
-      <c r="O86" s="8"/>
-      <c r="P86" s="8"/>
-      <c r="Q86" s="8"/>
-      <c r="R86" s="22"/>
-      <c r="S86" s="9"/>
-      <c r="T86" s="8"/>
-    </row>
-    <row r="87" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
-      <c r="I87" s="7"/>
-      <c r="J87" s="8"/>
-      <c r="K87" s="8"/>
-      <c r="L87" s="8"/>
-      <c r="M87" s="8"/>
-      <c r="N87" s="8"/>
-      <c r="O87" s="8"/>
-      <c r="P87" s="8"/>
-      <c r="Q87" s="8"/>
-      <c r="R87" s="22"/>
-      <c r="S87" s="9"/>
-      <c r="T87" s="8"/>
-    </row>
-    <row r="88" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="28">
+        <v>32</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="F61" s="31">
+        <v>45253</v>
+      </c>
+      <c r="G61" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="H61" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="I61" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="J61" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K61" s="33"/>
+      <c r="L61" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M61" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="N61" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="O61" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="P61" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q61" s="33"/>
+      <c r="R61" s="34"/>
+      <c r="S61" s="35"/>
+      <c r="T61" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="28">
+        <v>40</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="F62" s="31">
+        <v>45253</v>
+      </c>
+      <c r="G62" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="H62" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="I62" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="J62" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K62" s="33"/>
+      <c r="L62" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M62" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="N62" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="O62" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="P62" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q62" s="33"/>
+      <c r="R62" s="34"/>
+      <c r="S62" s="35"/>
+      <c r="T62" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="28">
+        <v>48</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D63" s="49" t="s">
+        <v>230</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="F63" s="31">
+        <v>45253</v>
+      </c>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K63" s="33"/>
+      <c r="L63" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M63" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="N63" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="O63" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="P63" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q63" s="33"/>
+      <c r="R63" s="34"/>
+      <c r="S63" s="35"/>
+      <c r="T63" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="28">
+        <v>147</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="E64" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="F64" s="31"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K64" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L64" s="33"/>
+      <c r="M64" s="33"/>
+      <c r="N64" s="33"/>
+      <c r="O64" s="33"/>
+      <c r="P64" s="33"/>
+      <c r="Q64" s="33"/>
+      <c r="R64" s="34"/>
+      <c r="S64" s="35"/>
+      <c r="T64" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="28">
+        <v>148</v>
+      </c>
+      <c r="B65" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D65" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="F65" s="31"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K65" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L65" s="33"/>
+      <c r="M65" s="33"/>
+      <c r="N65" s="33"/>
+      <c r="O65" s="33"/>
+      <c r="P65" s="33"/>
+      <c r="Q65" s="33"/>
+      <c r="R65" s="34"/>
+      <c r="S65" s="35"/>
+      <c r="T65" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="28">
+        <v>149</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="F66" s="31"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="32"/>
+      <c r="J66" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K66" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L66" s="33"/>
+      <c r="M66" s="33"/>
+      <c r="N66" s="33"/>
+      <c r="O66" s="33"/>
+      <c r="P66" s="33"/>
+      <c r="Q66" s="33"/>
+      <c r="R66" s="34"/>
+      <c r="S66" s="35"/>
+      <c r="T66" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="28">
+        <v>150</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D67" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="F67" s="31"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="32"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K67" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L67" s="33"/>
+      <c r="M67" s="33"/>
+      <c r="N67" s="33"/>
+      <c r="O67" s="33"/>
+      <c r="P67" s="33"/>
+      <c r="Q67" s="33"/>
+      <c r="R67" s="34"/>
+      <c r="S67" s="35"/>
+      <c r="T67" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="28">
+        <v>151</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="E68" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="F68" s="31"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32"/>
+      <c r="I68" s="32"/>
+      <c r="J68" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K68" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="L68" s="33"/>
+      <c r="M68" s="33"/>
+      <c r="N68" s="33"/>
+      <c r="O68" s="33"/>
+      <c r="P68" s="33"/>
+      <c r="Q68" s="33"/>
+      <c r="R68" s="34"/>
+      <c r="S68" s="35"/>
+      <c r="T68" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="28">
+        <v>152</v>
+      </c>
+      <c r="B69" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="F69" s="31">
+        <v>45253</v>
+      </c>
+      <c r="G69" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="H69" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="I69" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="J69" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K69" s="33"/>
+      <c r="L69" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M69" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="N69" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="O69" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="P69" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q69" s="33"/>
+      <c r="R69" s="34"/>
+      <c r="S69" s="35"/>
+      <c r="T69" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="28">
+        <v>153</v>
+      </c>
+      <c r="B70" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="F70" s="31">
+        <v>45253</v>
+      </c>
+      <c r="G70" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="H70" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="I70" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="J70" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K70" s="33"/>
+      <c r="L70" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M70" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="N70" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="O70" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="P70" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q70" s="33"/>
+      <c r="R70" s="34"/>
+      <c r="S70" s="35"/>
+      <c r="T70" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="28">
+        <v>154</v>
+      </c>
+      <c r="B71" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D71" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="F71" s="31"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="32"/>
+      <c r="J71" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K71" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="L71" s="33"/>
+      <c r="M71" s="33"/>
+      <c r="N71" s="33"/>
+      <c r="O71" s="33"/>
+      <c r="P71" s="33"/>
+      <c r="Q71" s="33"/>
+      <c r="R71" s="34"/>
+      <c r="S71" s="35"/>
+      <c r="T71" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="28">
+        <v>155</v>
+      </c>
+      <c r="B72" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D72" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="F72" s="31"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="32"/>
+      <c r="I72" s="32"/>
+      <c r="J72" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K72" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="L72" s="33"/>
+      <c r="M72" s="33"/>
+      <c r="N72" s="33"/>
+      <c r="O72" s="33"/>
+      <c r="P72" s="33"/>
+      <c r="Q72" s="33"/>
+      <c r="R72" s="34"/>
+      <c r="S72" s="35"/>
+      <c r="T72" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="28">
+        <v>156</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D73" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="F73" s="31"/>
+      <c r="G73" s="32"/>
+      <c r="H73" s="32"/>
+      <c r="I73" s="32"/>
+      <c r="J73" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K73" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="L73" s="33"/>
+      <c r="M73" s="33"/>
+      <c r="N73" s="33"/>
+      <c r="O73" s="33"/>
+      <c r="P73" s="33"/>
+      <c r="Q73" s="33"/>
+      <c r="R73" s="34"/>
+      <c r="S73" s="35"/>
+      <c r="T73" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="28">
+        <v>157</v>
+      </c>
+      <c r="B74" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D74" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="F74" s="31"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="32"/>
+      <c r="J74" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="K74" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L74" s="33"/>
+      <c r="M74" s="33"/>
+      <c r="N74" s="33"/>
+      <c r="O74" s="33"/>
+      <c r="P74" s="33"/>
+      <c r="Q74" s="33"/>
+      <c r="R74" s="34"/>
+      <c r="S74" s="35"/>
+      <c r="T74" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="28">
+        <v>158</v>
+      </c>
+      <c r="B75" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="F75" s="31"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="32"/>
+      <c r="I75" s="32"/>
+      <c r="J75" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="K75" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L75" s="33"/>
+      <c r="M75" s="33"/>
+      <c r="N75" s="33"/>
+      <c r="O75" s="33"/>
+      <c r="P75" s="33"/>
+      <c r="Q75" s="33"/>
+      <c r="R75" s="34"/>
+      <c r="S75" s="35"/>
+      <c r="T75" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="28">
+        <v>159</v>
+      </c>
+      <c r="B76" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D76" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="F76" s="31"/>
+      <c r="G76" s="32"/>
+      <c r="H76" s="32"/>
+      <c r="I76" s="32"/>
+      <c r="J76" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="K76" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L76" s="33"/>
+      <c r="M76" s="33"/>
+      <c r="N76" s="33"/>
+      <c r="O76" s="33"/>
+      <c r="P76" s="33"/>
+      <c r="Q76" s="33"/>
+      <c r="R76" s="34"/>
+      <c r="S76" s="35"/>
+      <c r="T76" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="28">
+        <v>160</v>
+      </c>
+      <c r="B77" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="F77" s="31"/>
+      <c r="G77" s="32"/>
+      <c r="H77" s="32"/>
+      <c r="I77" s="32"/>
+      <c r="J77" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K77" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="L77" s="33"/>
+      <c r="M77" s="33"/>
+      <c r="N77" s="33"/>
+      <c r="O77" s="33"/>
+      <c r="P77" s="33"/>
+      <c r="Q77" s="33"/>
+      <c r="R77" s="34"/>
+      <c r="S77" s="35"/>
+      <c r="T77" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="28">
+        <v>161</v>
+      </c>
+      <c r="B78" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C78" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="F78" s="31"/>
+      <c r="G78" s="32"/>
+      <c r="H78" s="32"/>
+      <c r="I78" s="32"/>
+      <c r="J78" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K78" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="L78" s="33"/>
+      <c r="M78" s="33"/>
+      <c r="N78" s="33"/>
+      <c r="O78" s="33"/>
+      <c r="P78" s="33"/>
+      <c r="Q78" s="33"/>
+      <c r="R78" s="34"/>
+      <c r="S78" s="35"/>
+      <c r="T78" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="28">
+        <v>162</v>
+      </c>
+      <c r="B79" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D79" s="29" t="s">
+        <v>262</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="F79" s="31"/>
+      <c r="G79" s="32"/>
+      <c r="H79" s="32"/>
+      <c r="I79" s="32"/>
+      <c r="J79" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K79" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L79" s="33"/>
+      <c r="M79" s="33"/>
+      <c r="N79" s="33"/>
+      <c r="O79" s="33"/>
+      <c r="P79" s="33"/>
+      <c r="Q79" s="33"/>
+      <c r="R79" s="34"/>
+      <c r="S79" s="35"/>
+      <c r="T79" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="28">
+        <v>163</v>
+      </c>
+      <c r="B80" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D80" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="F80" s="31"/>
+      <c r="G80" s="32"/>
+      <c r="H80" s="32"/>
+      <c r="I80" s="32"/>
+      <c r="J80" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K80" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="L80" s="33"/>
+      <c r="M80" s="33"/>
+      <c r="N80" s="33"/>
+      <c r="O80" s="33"/>
+      <c r="P80" s="33"/>
+      <c r="Q80" s="33"/>
+      <c r="R80" s="34"/>
+      <c r="S80" s="35"/>
+      <c r="T80" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="28">
+        <v>164</v>
+      </c>
+      <c r="B81" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="F81" s="31"/>
+      <c r="G81" s="32"/>
+      <c r="H81" s="32"/>
+      <c r="I81" s="32"/>
+      <c r="J81" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K81" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L81" s="33"/>
+      <c r="M81" s="33"/>
+      <c r="N81" s="33"/>
+      <c r="O81" s="33"/>
+      <c r="P81" s="33"/>
+      <c r="Q81" s="33"/>
+      <c r="R81" s="34"/>
+      <c r="S81" s="35"/>
+      <c r="T81" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="28">
+        <v>165</v>
+      </c>
+      <c r="B82" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D82" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="F82" s="31"/>
+      <c r="G82" s="32"/>
+      <c r="H82" s="32"/>
+      <c r="I82" s="32"/>
+      <c r="J82" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K82" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L82" s="33"/>
+      <c r="M82" s="33"/>
+      <c r="N82" s="33"/>
+      <c r="O82" s="33"/>
+      <c r="P82" s="33"/>
+      <c r="Q82" s="33"/>
+      <c r="R82" s="34"/>
+      <c r="S82" s="35"/>
+      <c r="T82" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="28">
+        <v>166</v>
+      </c>
+      <c r="B83" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D83" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="F83" s="31"/>
+      <c r="G83" s="32"/>
+      <c r="H83" s="32"/>
+      <c r="I83" s="32"/>
+      <c r="J83" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K83" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L83" s="33"/>
+      <c r="M83" s="33"/>
+      <c r="N83" s="33"/>
+      <c r="O83" s="33"/>
+      <c r="P83" s="33"/>
+      <c r="Q83" s="33"/>
+      <c r="R83" s="34"/>
+      <c r="S83" s="35"/>
+      <c r="T83" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="28">
+        <v>167</v>
+      </c>
+      <c r="B84" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D84" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="F84" s="31"/>
+      <c r="G84" s="32"/>
+      <c r="H84" s="32"/>
+      <c r="I84" s="32"/>
+      <c r="J84" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K84" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L84" s="33"/>
+      <c r="M84" s="33"/>
+      <c r="N84" s="33"/>
+      <c r="O84" s="33"/>
+      <c r="P84" s="33"/>
+      <c r="Q84" s="33"/>
+      <c r="R84" s="34"/>
+      <c r="S84" s="35"/>
+      <c r="T84" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="28">
+        <v>168</v>
+      </c>
+      <c r="B85" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D85" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="F85" s="31"/>
+      <c r="G85" s="32"/>
+      <c r="H85" s="32"/>
+      <c r="I85" s="32"/>
+      <c r="J85" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K85" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L85" s="33"/>
+      <c r="M85" s="33"/>
+      <c r="N85" s="33"/>
+      <c r="O85" s="33"/>
+      <c r="P85" s="33"/>
+      <c r="Q85" s="33"/>
+      <c r="R85" s="34"/>
+      <c r="S85" s="35"/>
+      <c r="T85" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="28">
+        <v>169</v>
+      </c>
+      <c r="B86" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="F86" s="31"/>
+      <c r="G86" s="32"/>
+      <c r="H86" s="32"/>
+      <c r="I86" s="32"/>
+      <c r="J86" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K86" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="L86" s="33"/>
+      <c r="M86" s="33"/>
+      <c r="N86" s="33"/>
+      <c r="O86" s="33"/>
+      <c r="P86" s="33"/>
+      <c r="Q86" s="33"/>
+      <c r="R86" s="34"/>
+      <c r="S86" s="35"/>
+      <c r="T86" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" ht="165" x14ac:dyDescent="0.25">
+      <c r="A87" s="28">
+        <v>374</v>
+      </c>
+      <c r="B87" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D87" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="E87" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="F87" s="31">
+        <v>45253</v>
+      </c>
+      <c r="G87" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="H87" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="I87" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="J87" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K87" s="33"/>
+      <c r="L87" s="33"/>
+      <c r="M87" s="33"/>
+      <c r="N87" s="33"/>
+      <c r="O87" s="33"/>
+      <c r="P87" s="33"/>
+      <c r="Q87" s="33"/>
+      <c r="R87" s="34"/>
+      <c r="S87" s="35"/>
+      <c r="T87" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
@@ -4797,7 +5843,7 @@
       <c r="S88" s="9"/>
       <c r="T88" s="8"/>
     </row>
-    <row r="89" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
@@ -4814,7 +5860,7 @@
       <c r="S89" s="9"/>
       <c r="T89" s="8"/>
     </row>
-    <row r="90" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
@@ -4831,7 +5877,7 @@
       <c r="S90" s="9"/>
       <c r="T90" s="8"/>
     </row>
-    <row r="91" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
@@ -4848,7 +5894,7 @@
       <c r="S91" s="9"/>
       <c r="T91" s="8"/>
     </row>
-    <row r="92" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
@@ -4865,7 +5911,7 @@
       <c r="S92" s="9"/>
       <c r="T92" s="8"/>
     </row>
-    <row r="93" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
@@ -4882,7 +5928,7 @@
       <c r="S93" s="9"/>
       <c r="T93" s="8"/>
     </row>
-    <row r="94" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
@@ -4899,7 +5945,7 @@
       <c r="S94" s="9"/>
       <c r="T94" s="8"/>
     </row>
-    <row r="95" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
@@ -4916,7 +5962,7 @@
       <c r="S95" s="9"/>
       <c r="T95" s="8"/>
     </row>
-    <row r="96" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
@@ -18687,7 +19733,7 @@
       <c r="T905" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T60" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A9:T87" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -18707,13 +19753,13 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O1:O8 L1:M8 L10:M1048576 O10:O1048576</xm:sqref>
+          <xm:sqref>O1:O8 L1:M8 O88:O1048576 O10:O60 L10:M60 L88:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J10:J60</xm:sqref>
+          <xm:sqref>J10:J60 J74:J76</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>

</xml_diff>

<commit_message>
Aggiunti ID 369 e 373.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
+++ b/GATEWAY/A1#111S3K00000000/S3K_SPA/JHIS/23.01.01/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lavoro\FSE\Accreditamento\GitHub\GATEWAY\A1#111S3K00000000\S3K_SPA\JHIS\23.01.01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005E25C9-22C4-443E-8863-6047831E6DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC8B304-9D59-459C-9957-867605A290DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,21 @@
     <sheet name="Sheet1" sheetId="4" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$9:$T$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$9:$T$89</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mhXj7RfszpgZKzxg8oD/Tet7lb94w=="/>
     </ext>
@@ -60,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="310">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -1374,6 +1385,40 @@
   </si>
   <si>
     <t>Impossibile contattare l'FSE"</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_VPS_CT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2024-01-09T14:41:42Z</t>
+  </si>
+  <si>
+    <t>3f69117ef135ae1e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.bc59104422807a7cb0f44cc5db474da21de3fafc69db09e707093d4f0eab50d5.51ec4ae202^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-01-09T17:44:17Z</t>
+  </si>
+  <si>
+    <t>5289ea02744f3053</t>
+  </si>
+  <si>
+    <t>workflowInstanceId":"2.16.840.1.113883.2.9.2.100.4.4.ecc4f67fa00bbd32757bace6843eac219e8195f8d189d9525cd9c130f9a276b8.12b77b7bae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1698,7 +1743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1859,12 +1904,9 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -2233,13 +2275,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T905"/>
+  <dimension ref="A1:T907"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4838,7 +4880,7 @@
       <c r="C63" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="D63" s="49" t="s">
+      <c r="D63" s="29" t="s">
         <v>230</v>
       </c>
       <c r="E63" s="30" t="s">
@@ -5782,33 +5824,33 @@
         <v>133</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="165" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="28">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B87" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C87" s="29" t="s">
-        <v>225</v>
+        <v>18</v>
       </c>
       <c r="D87" s="29" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="F87" s="31">
-        <v>45253</v>
+        <v>45300</v>
       </c>
       <c r="G87" s="32" t="s">
-        <v>286</v>
+        <v>307</v>
       </c>
       <c r="H87" s="32" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="I87" s="32" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="J87" s="33" t="s">
         <v>36</v>
@@ -5826,39 +5868,93 @@
         <v>132</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F88" s="7"/>
-      <c r="G88" s="7"/>
-      <c r="H88" s="7"/>
-      <c r="I88" s="7"/>
-      <c r="J88" s="8"/>
-      <c r="K88" s="8"/>
-      <c r="L88" s="8"/>
-      <c r="M88" s="8"/>
-      <c r="N88" s="8"/>
-      <c r="O88" s="8"/>
-      <c r="P88" s="8"/>
-      <c r="Q88" s="8"/>
-      <c r="R88" s="22"/>
-      <c r="S88" s="9"/>
-      <c r="T88" s="8"/>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
-      <c r="I89" s="7"/>
-      <c r="J89" s="8"/>
-      <c r="K89" s="8"/>
-      <c r="L89" s="8"/>
-      <c r="M89" s="8"/>
-      <c r="N89" s="8"/>
-      <c r="O89" s="8"/>
-      <c r="P89" s="8"/>
-      <c r="Q89" s="8"/>
-      <c r="R89" s="22"/>
-      <c r="S89" s="9"/>
-      <c r="T89" s="8"/>
+    <row r="88" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="28">
+        <v>373</v>
+      </c>
+      <c r="B88" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D88" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="E88" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="F88" s="31">
+        <v>45300</v>
+      </c>
+      <c r="G88" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="H88" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="I88" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="J88" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K88" s="33"/>
+      <c r="L88" s="33"/>
+      <c r="M88" s="33"/>
+      <c r="N88" s="33"/>
+      <c r="O88" s="33"/>
+      <c r="P88" s="33"/>
+      <c r="Q88" s="33"/>
+      <c r="R88" s="34"/>
+      <c r="S88" s="35"/>
+      <c r="T88" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" ht="165" x14ac:dyDescent="0.25">
+      <c r="A89" s="28">
+        <v>374</v>
+      </c>
+      <c r="B89" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D89" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="E89" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="F89" s="31">
+        <v>45253</v>
+      </c>
+      <c r="G89" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="H89" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="I89" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="J89" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K89" s="33"/>
+      <c r="L89" s="33"/>
+      <c r="M89" s="33"/>
+      <c r="N89" s="33"/>
+      <c r="O89" s="33"/>
+      <c r="P89" s="33"/>
+      <c r="Q89" s="33"/>
+      <c r="R89" s="34"/>
+      <c r="S89" s="35"/>
+      <c r="T89" s="36" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F90" s="7"/>
@@ -19732,8 +19828,42 @@
       <c r="S905" s="9"/>
       <c r="T905" s="8"/>
     </row>
+    <row r="906" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F906" s="7"/>
+      <c r="G906" s="7"/>
+      <c r="H906" s="7"/>
+      <c r="I906" s="7"/>
+      <c r="J906" s="8"/>
+      <c r="K906" s="8"/>
+      <c r="L906" s="8"/>
+      <c r="M906" s="8"/>
+      <c r="N906" s="8"/>
+      <c r="O906" s="8"/>
+      <c r="P906" s="8"/>
+      <c r="Q906" s="8"/>
+      <c r="R906" s="22"/>
+      <c r="S906" s="9"/>
+      <c r="T906" s="8"/>
+    </row>
+    <row r="907" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F907" s="7"/>
+      <c r="G907" s="7"/>
+      <c r="H907" s="7"/>
+      <c r="I907" s="7"/>
+      <c r="J907" s="8"/>
+      <c r="K907" s="8"/>
+      <c r="L907" s="8"/>
+      <c r="M907" s="8"/>
+      <c r="N907" s="8"/>
+      <c r="O907" s="8"/>
+      <c r="P907" s="8"/>
+      <c r="Q907" s="8"/>
+      <c r="R907" s="22"/>
+      <c r="S907" s="9"/>
+      <c r="T907" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A9:T87" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A9:T89" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -19753,7 +19883,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O1:O8 L1:M8 O88:O1048576 O10:O60 L10:M60 L88:M1048576</xm:sqref>
+          <xm:sqref>O1:O8 L1:M8 O90:O1048576 O10:O60 L10:M60 L90:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
@@ -20821,6 +20951,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -21051,27 +21201,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21090,31 +21245,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>